<commit_message>
Question: add faq question type
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/topics.xlsx
+++ b/lib/samples/assets/csv/topics.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>code</t>
   </si>
@@ -36,18 +36,33 @@
     <t>ការមានរដូវមិនទៀងទាត់?</t>
   </si>
   <si>
+    <t>topic_03</t>
+  </si>
+  <si>
+    <t>តើសុខភាពយុវជនជាអ្វី?</t>
+  </si>
+  <si>
     <t>topic_code</t>
   </si>
   <si>
     <t>hint</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
     <t>question_01_01</t>
   </si>
   <si>
     <t>ខ្ញុំមានកូនដោយមិនចង់បាន តើគួរធ្វើបែបណា?</t>
   </si>
   <si>
+    <t>selectone</t>
+  </si>
+  <si>
     <t>question_02_01</t>
   </si>
   <si>
@@ -58,6 +73,15 @@
   </si>
   <si>
     <t>តើរដូវចុងក្រោយរបស់អ្នកមានរយះពេលប៉ុន្មានថ្ងៃដែរ?</t>
+  </si>
+  <si>
+    <t>question_03_01</t>
+  </si>
+  <si>
+    <t>faq</t>
+  </si>
+  <si>
+    <t>ជាប្រភពព័ត៌មានជាសាធារណៈមួយដែលបង្កើតឡើងសម្រាប់ប្រើប្រាស់ដោយមិនមានការគិតថ្លៃ និងមានបំណងឲ្យប្រើប្រាស់ស្របតាមគោលបំណងរបស់អ៊ែប</t>
   </si>
   <si>
     <t>question_code</t>
@@ -106,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -131,6 +155,11 @@
       <sz val="11.0"/>
       <color rgb="FF172B4D"/>
       <name val="-apple-system"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF212529"/>
+      <name val="Nunito"/>
     </font>
     <font>
       <b/>
@@ -175,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -198,24 +227,27 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -475,6 +507,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -491,12 +531,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="36.88"/>
-    <col customWidth="1" min="6" max="6" width="15.38"/>
+    <col customWidth="1" min="7" max="7" width="15.38"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -505,25 +545,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="G1" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H1" s="7"/>
       <c r="I1" s="8"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -531,10 +579,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -542,10 +593,30 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -570,70 +641,70 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="10"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>19</v>
+      <c r="D2" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -641,30 +712,30 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>